<commit_message>
merging branches for current cad status
</commit_message>
<xml_diff>
--- a/documentation/Partslist.xlsx
+++ b/documentation/Partslist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Just Data\Projects\DrAI\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499C8518-82BB-4E63-A7CB-527519D11B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E52E894-F801-4A08-9B7B-66BD334EE8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{5FB60B51-FE56-4ED2-81C0-A7A75F33C42C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -202,24 +202,6 @@
   </si>
   <si>
     <t>Misc. Cable management</t>
-  </si>
-  <si>
-    <t>E_U2-5</t>
-  </si>
-  <si>
-    <t>U1_U1-U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stepper Controller </t>
-  </si>
-  <si>
-    <t>https://www.amazon.de/-/en/dp/B093WLW6MT?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
-  </si>
-  <si>
-    <t>Exact</t>
-  </si>
-  <si>
-    <t>https://www.amazon.de/gp/product/B08G1VLQCK/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -229,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +292,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -410,29 +385,24 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27" customBuiltin="1"/>
@@ -443,33 +413,7 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b val="0"/>
@@ -506,42 +450,26 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -688,24 +616,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -874,6 +784,24 @@
           <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -889,21 +817,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42AF2102-102D-4103-A6D5-24FFCC2EB361}" name="Parts_List" displayName="Parts_List" ref="B4:J22" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="B4:J21" xr:uid="{42AF2102-102D-4103-A6D5-24FFCC2EB361}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3BE58933-244B-4B76-A9EB-11B926ECBCA0}" name="ID" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E0203CEB-6877-431A-A00B-149F01336670}" name="Circuit" dataDxfId="16" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BE505530-5D7B-4D7D-86F8-A899EE6E35B1}" name="General" dataDxfId="15" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{CBFAF02A-C11C-4B88-B577-B4D95BA852EE}" name="Name" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{B35FCA72-BF49-4118-9E2E-03767F2FB370}" name="Link" dataDxfId="13" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{64F2A74F-AAAC-4877-ACDE-B0E917561767}" name="Quan." dataDxfId="12" totalsRowDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{883FFC3A-5BBC-44BC-AE6E-879B0D5D5897}" name="Single" dataDxfId="11" totalsRowDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{6DB48C97-28C0-4DD2-A5F4-144635F5DF19}" name="Total" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42AF2102-102D-4103-A6D5-24FFCC2EB361}" name="Parts_List" displayName="Parts_List" ref="C4:J21" totalsRowCount="1" headerRowDxfId="19" dataDxfId="20">
+  <autoFilter ref="C4:J20" xr:uid="{42AF2102-102D-4103-A6D5-24FFCC2EB361}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3BE58933-244B-4B76-A9EB-11B926ECBCA0}" name="ID" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{E0203CEB-6877-431A-A00B-149F01336670}" name="Circuit" dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BE505530-5D7B-4D7D-86F8-A899EE6E35B1}" name="General" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{CBFAF02A-C11C-4B88-B577-B4D95BA852EE}" name="Name" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{B35FCA72-BF49-4118-9E2E-03767F2FB370}" name="Link" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{64F2A74F-AAAC-4877-ACDE-B0E917561767}" name="Quan." dataDxfId="10" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{883FFC3A-5BBC-44BC-AE6E-879B0D5D5897}" name="Single" dataDxfId="9" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{6DB48C97-28C0-4DD2-A5F4-144635F5DF19}" name="Total" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{7B7B325B-4986-4F6D-AB62-0703E51F55C2}" name="Exact" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="0" dataCellStyle="Currency" totalsRowCellStyle="Currency">
-      <totalsRowFormula>SUBTOTAL(109,Parts_List[Exact])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -911,8 +836,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AFDBE559-D616-423A-A4E3-62452F03AD98}" name="Status" displayName="Status" ref="L11:L15" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="L11:L15" xr:uid="{AFDBE559-D616-423A-A4E3-62452F03AD98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AFDBE559-D616-423A-A4E3-62452F03AD98}" name="Status" displayName="Status" ref="M4:M8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17">
+  <autoFilter ref="M4:M8" xr:uid="{AFDBE559-D616-423A-A4E3-62452F03AD98}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7EDE620A-B8A0-4DA2-AC1A-8EBD34ED5AB4}" name="Status" dataDxfId="18"/>
   </tableColumns>
@@ -1217,537 +1142,474 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2F50A-8AAE-4C9A-8947-DA205D7B5632}">
-  <dimension ref="B2:L25"/>
+  <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.08984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.36328125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="10.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="13.26953125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="11.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.36328125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="1"/>
+    <col min="13" max="13" width="13.26953125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="10">
+      <c r="M4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <v>60</v>
       </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>60</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="J5" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>60</v>
       </c>
-      <c r="J5" s="3">
-        <v>51.02</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="10">
+      <c r="M5" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="C6" s="10">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="6">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="4">
         <v>25</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>25</v>
       </c>
-      <c r="J6" s="3">
-        <v>8.07</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="8">
+      <c r="M6" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="10">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="4">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="6">
         <v>4</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="4">
         <v>10</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>40</v>
       </c>
-      <c r="J7" s="3">
-        <v>32.99</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
+      <c r="M7" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="10">
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4</v>
-      </c>
-      <c r="H8" s="3">
-        <v>18</v>
-      </c>
-      <c r="I8" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>72</v>
-      </c>
-      <c r="J8" s="3">
-        <v>51.42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="9">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H8" s="6">
         <v>2</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I8" s="4">
         <v>6</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J8" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>12</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="14">
+      <c r="M8" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16">
+      <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="H10" s="17">
-        <v>0</v>
-      </c>
-      <c r="I10" s="17">
+      <c r="I9" s="4">
+        <v>35</v>
+      </c>
+      <c r="J9" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="C10" s="10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>30</v>
+      </c>
+      <c r="J10" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="13">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C12" s="10">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="10">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>5</v>
+      </c>
+      <c r="J13" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="13">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="6">
+        <v>4</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="10">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>15</v>
+      </c>
+      <c r="J15" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="12">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>50</v>
+      </c>
+      <c r="J16" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="13">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>30</v>
+      </c>
+      <c r="J17" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>80</v>
+      </c>
+      <c r="J18" s="4">
+        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>0</v>
       </c>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="2:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="8">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>30</v>
-      </c>
-      <c r="I11" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>30</v>
-      </c>
-      <c r="J11" s="3">
-        <v>39.159999999999997</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
-        <v>7</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16">
-        <v>1</v>
-      </c>
-      <c r="H12" s="17">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H20" s="6"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4">
         <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
         <v>0</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="L12" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>10</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="L13" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="7">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="4">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3">
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>10</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="L14" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="10">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="4">
-        <v>4</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I15" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>2</v>
-      </c>
-      <c r="J15" s="3"/>
-      <c r="L15" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="7">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>15</v>
-      </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3">
-        <v>50</v>
-      </c>
-      <c r="I17" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>50</v>
-      </c>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>30</v>
-      </c>
-      <c r="I18" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>30</v>
-      </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="9">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="4">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>80</v>
-      </c>
-      <c r="I19" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>80</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
-        <v>15</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G21" s="4"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <f>Parts_List[[#This Row],[Quan.]]*Parts_List[[#This Row],[Single]]</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="7">
         <f>SUBTOTAL(109,Parts_List[Total])</f>
-        <v>436</v>
-      </c>
-      <c r="J22" s="19">
-        <f>SUBTOTAL(109,Parts_List[Exact])</f>
-        <v>182.66</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="J22" s="1">
         <v>1.2</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="1" t="s">
+    <row r="23" spans="3:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="11">
-        <f>Parts_List[[#Totals],[Total]]*I23</f>
-        <v>523.19999999999993</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="J23" s="14">
+        <f>Parts_List[[#Totals],[Total]]*J22</f>
+        <v>490.79999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="C2:E3"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{533C9938-EF60-47B6-A645-D0231457AD24}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{0A1D004D-434D-47D2-8E11-9097C9D7645A}"/>
-    <hyperlink ref="F9" r:id="rId3" xr:uid="{CD68806C-4D50-454C-903B-D76EF2A60FAE}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{C79DD022-65DF-49DC-8DA6-7E26460A5592}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{B5BE6B29-DB17-4FA8-853F-BAB0D814ED59}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{9DA8CB82-F93B-4B12-9187-8281EB04A27B}"/>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{533C9938-EF60-47B6-A645-D0231457AD24}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{0A1D004D-434D-47D2-8E11-9097C9D7645A}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{CD68806C-4D50-454C-903B-D76EF2A60FAE}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{C79DD022-65DF-49DC-8DA6-7E26460A5592}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId5"/>
   <tableParts count="2">
-    <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>